<commit_message>
update names on rubric
</commit_message>
<xml_diff>
--- a/Rubric.xlsx
+++ b/Rubric.xlsx
@@ -1,39 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bblanchard006/Desktop/SMU/MLI/Fall 2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tina/Documents/School/ML1/SMUMSDS-ML1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670D4D1E-2A33-AB4E-9441-8BC0521D892C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE260CA-661E-CD44-A355-52EB6C94AC22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1080" windowWidth="27240" windowHeight="18540" xr2:uid="{BF90F522-138A-0945-890E-4BF33CEC6E34}"/>
+    <workbookView xWindow="1300" yWindow="460" windowWidth="27240" windowHeight="16720" xr2:uid="{BF90F522-138A-0945-890E-4BF33CEC6E34}"/>
   </bookViews>
   <sheets>
     <sheet name="Group #" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Rubric</t>
   </si>
@@ -366,6 +358,18 @@
       </rPr>
       <t xml:space="preserve"> algorithm? Be specific.</t>
     </r>
+  </si>
+  <si>
+    <t>Fabio</t>
+  </si>
+  <si>
+    <t>Ellen</t>
+  </si>
+  <si>
+    <t>Paritosh</t>
+  </si>
+  <si>
+    <t>Tina</t>
   </si>
 </sst>
 </file>
@@ -814,13 +818,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F1D61A-62F8-D049-9179-45C2A4893D1C}">
-  <dimension ref="B1:F12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,7 +838,7 @@
     <col min="7" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -848,7 +852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -866,7 +870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
@@ -881,7 +885,10 @@
       </c>
       <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="2:6" ht="119" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -894,7 +901,10 @@
       <c r="E4" s="9"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="2:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -907,7 +917,10 @@
       <c r="E5" s="9"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -920,7 +933,10 @@
       <c r="E6" s="9"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
@@ -933,7 +949,10 @@
       <c r="E7" s="9"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
@@ -946,7 +965,10 @@
       <c r="E8" s="9"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
@@ -959,7 +981,10 @@
       <c r="E9" s="9"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
@@ -972,7 +997,10 @@
       <c r="E10" s="9"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="2:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
@@ -985,7 +1013,7 @@
       <c r="E11" s="9"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>

</xml_diff>